<commit_message>
Create modul fill_table, create class DataRM
</commit_message>
<xml_diff>
--- a/help/add fields rg2.xlsx
+++ b/help/add fields rg2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\rastr_add\help\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\rastr_add2\help\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D878C31-5F63-4923-A0B6-198201E25D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76401E22-93A8-4075-9B6C-0856E3CE55A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="872" activeTab="6" xr2:uid="{7CA5A748-59CE-4C69-98CB-7D08DFB7A4A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="872" activeTab="5" xr2:uid="{7CA5A748-59CE-4C69-98CB-7D08DFB7A4A1}"/>
   </bookViews>
   <sheets>
     <sheet name="area" sheetId="62" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="149">
   <si>
     <t>Имя</t>
   </si>
@@ -1453,7 +1453,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1606,7 +1606,7 @@
         <v>75</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -1696,19 +1696,12 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="1" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="24.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.140625" customWidth="1"/>
@@ -1846,10 +1839,10 @@
     </row>
     <row r="7" spans="1:17" s="1" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -1938,8 +1931,8 @@
   </sheetPr>
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2252,7 +2245,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD19"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2589,13 +2582,13 @@
   <sheetPr codeName="Лист5">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3013,6 +3006,31 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:17" s="11" customFormat="1">
+      <c r="A14" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23">
+        <v>3</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3028,9 +3046,9 @@
   </sheetPr>
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q21" sqref="A21:Q21"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3733,11 +3751,11 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>